<commit_message>
Added data output capabilities.
As the application searches, it will now output its findings to the output excel document.

Still needs some work to support multiple finds. But the groundwork is there.
</commit_message>
<xml_diff>
--- a/jobSearchTerms.xlsx
+++ b/jobSearchTerms.xlsx
@@ -37,52 +37,52 @@
     <t xml:space="preserve">paid training</t>
   </si>
   <si>
+    <t xml:space="preserve">ga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">will train</t>
+  </si>
+  <si>
+    <t xml:space="preserve">portland, or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">programmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">willing to train</t>
+  </si>
+  <si>
+    <t xml:space="preserve">austin, tx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inexperienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seattle, wa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no experience necessary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on the job training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">va</t>
+  </si>
+  <si>
     <t xml:space="preserve">charlotte, nc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cnc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">will train</t>
-  </si>
-  <si>
-    <t xml:space="preserve">portland, or</t>
-  </si>
-  <si>
-    <t xml:space="preserve">programmer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">willing to train</t>
-  </si>
-  <si>
-    <t xml:space="preserve">austin, tx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inexperienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seattle, wa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no experience necessary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">on the job trainiing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">va</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ga</t>
   </si>
   <si>
     <t xml:space="preserve">us</t>
@@ -184,7 +184,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>